<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-16 13:20:24
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -81,7 +81,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -103,6 +103,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -486,7 +489,7 @@
     <col width="10" customWidth="1" min="6" max="6"/>
     <col width="50" customWidth="1" min="7" max="7"/>
     <col width="10" customWidth="1" min="8" max="8"/>
-    <col width="10" customWidth="1" min="9" max="9"/>
+    <col width="14" customWidth="1" min="9" max="9"/>
     <col width="22" customWidth="1" min="11" max="11"/>
     <col width="8" customWidth="1" min="12" max="12"/>
     <col width="18" customWidth="1" min="13" max="13"/>
@@ -578,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -630,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -855,7 +858,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -906,7 +909,7 @@
         </is>
       </c>
       <c r="L8" s="5" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9">
@@ -1278,7 +1281,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1311,10 +1314,10 @@
         <v>7</v>
       </c>
       <c r="P15" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q15" s="5" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="R15" s="5" t="inlineStr">
         <is>
@@ -1960,45 +1963,45 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B29" s="4" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C29" s="4" t="inlineStr">
+      <c r="A29" s="9" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B29" s="9" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C29" s="9" t="inlineStr">
         <is>
           <t>PHYSIOLOGY</t>
         </is>
       </c>
-      <c r="D29" s="4" t="inlineStr">
+      <c r="D29" s="9" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E29" s="4" t="inlineStr">
+      <c r="E29" s="9" t="inlineStr">
         <is>
           <t>16/11/2025</t>
         </is>
       </c>
-      <c r="F29" s="4" t="inlineStr">
+      <c r="F29" s="9" t="inlineStr">
         <is>
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G29" s="4" t="inlineStr"/>
-      <c r="H29" s="4" t="inlineStr">
-        <is>
-          <t>0/251</t>
-        </is>
-      </c>
-      <c r="I29" s="4" t="inlineStr">
-        <is>
-          <t>Pending</t>
+      <c r="G29" s="9" t="inlineStr"/>
+      <c r="H29" s="9" t="inlineStr">
+        <is>
+          <t>0/251</t>
+        </is>
+      </c>
+      <c r="I29" s="9" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-16 14:12:04
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System</t>
+          <t>asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-16 15:13:08
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, System</t>
+          <t>Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-16 16:15:54
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>System, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>eman.tantawi@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-16 17:12:24
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>eman.tantawi@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>System, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -945,7 +945,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-16 18:19:18
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-16 19:10:46
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
+          <t>gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System</t>
+          <t>eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-16 20:15:29
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System</t>
+          <t>gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System</t>
+          <t>asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -945,7 +945,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-16 21:12:17
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>System, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System</t>
+          <t>asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-16 22:13:27
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -945,7 +945,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-16 23:13:23
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System</t>
+          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg</t>
+          <t>eman.tantawi@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-17 01:10:36
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>eman.tantawi@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>System, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-17 03:11:58
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-17 04:21:24
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System</t>
+          <t>Veronia.rafat@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-17 05:15:37
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-17 06:23:37
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
+          <t>gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
+          <t>Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -1948,7 +1948,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-17 07:15:31
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -96,6 +96,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -103,9 +106,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, servinaz@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg</t>
+          <t>eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -858,7 +858,7 @@
         </is>
       </c>
       <c r="L7" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -909,7 +909,7 @@
         </is>
       </c>
       <c r="L8" s="5" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9">
@@ -945,7 +945,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -970,45 +970,45 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B10" s="4" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C10" s="4" t="inlineStr">
+      <c r="A10" s="6" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B10" s="6" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C10" s="6" t="inlineStr">
         <is>
           <t>HISTOLOGY</t>
         </is>
       </c>
-      <c r="D10" s="4" t="inlineStr">
+      <c r="D10" s="6" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E10" s="4" t="inlineStr">
+      <c r="E10" s="6" t="inlineStr">
         <is>
           <t>17/11/2025</t>
         </is>
       </c>
-      <c r="F10" s="4" t="inlineStr">
+      <c r="F10" s="6" t="inlineStr">
         <is>
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G10" s="4" t="inlineStr"/>
-      <c r="H10" s="4" t="inlineStr">
-        <is>
-          <t>0/251</t>
-        </is>
-      </c>
-      <c r="I10" s="4" t="inlineStr">
-        <is>
-          <t>Pending</t>
+      <c r="G10" s="6" t="inlineStr"/>
+      <c r="H10" s="6" t="inlineStr">
+        <is>
+          <t>0/251</t>
+        </is>
+      </c>
+      <c r="I10" s="6" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
       <c r="K10" s="5" t="inlineStr">
@@ -1281,7 +1281,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1314,10 +1314,10 @@
         <v>7</v>
       </c>
       <c r="P15" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q15" s="5" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="R15" s="5" t="inlineStr">
         <is>
@@ -1569,7 +1569,7 @@
           <t>Recorded</t>
         </is>
       </c>
-      <c r="L20" s="6" t="inlineStr">
+      <c r="L20" s="7" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -1627,7 +1627,7 @@
           <t>Not Recorded</t>
         </is>
       </c>
-      <c r="L21" s="7" t="inlineStr">
+      <c r="L21" s="8" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -1685,7 +1685,7 @@
           <t>Pending</t>
         </is>
       </c>
-      <c r="L22" s="8" t="inlineStr">
+      <c r="L22" s="9" t="inlineStr">
         <is>
           <t>Yellow</t>
         </is>
@@ -1948,7 +1948,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">
@@ -1963,43 +1963,43 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="9" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B29" s="9" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C29" s="9" t="inlineStr">
+      <c r="A29" s="6" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B29" s="6" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C29" s="6" t="inlineStr">
         <is>
           <t>PHYSIOLOGY</t>
         </is>
       </c>
-      <c r="D29" s="9" t="inlineStr">
+      <c r="D29" s="6" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E29" s="9" t="inlineStr">
+      <c r="E29" s="6" t="inlineStr">
         <is>
           <t>16/11/2025</t>
         </is>
       </c>
-      <c r="F29" s="9" t="inlineStr">
+      <c r="F29" s="6" t="inlineStr">
         <is>
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G29" s="9" t="inlineStr"/>
-      <c r="H29" s="9" t="inlineStr">
-        <is>
-          <t>0/251</t>
-        </is>
-      </c>
-      <c r="I29" s="9" t="inlineStr">
+      <c r="G29" s="6" t="inlineStr"/>
+      <c r="H29" s="6" t="inlineStr">
+        <is>
+          <t>0/251</t>
+        </is>
+      </c>
+      <c r="I29" s="6" t="inlineStr">
         <is>
           <t>Not Recorded</t>
         </is>

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-17 09:19:44
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -90,10 +90,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, System</t>
+          <t>servinaz@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg</t>
+          <t>eman.tantawi@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -658,258 +658,262 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B4" s="4" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C4" s="4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>ANATOMY</t>
         </is>
       </c>
-      <c r="D4" s="4" t="inlineStr">
+      <c r="D4" s="2" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="E4" s="4" t="inlineStr">
+      <c r="E4" s="2" t="inlineStr">
         <is>
           <t>17/11/2025</t>
         </is>
       </c>
-      <c r="F4" s="4" t="inlineStr">
+      <c r="F4" s="2" t="inlineStr">
         <is>
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G4" s="4" t="inlineStr"/>
-      <c r="H4" s="4" t="inlineStr">
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>majorelle.magdy@med.asu.edu.eg</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="inlineStr">
+        <is>
+          <t>16/251</t>
+        </is>
+      </c>
+      <c r="I4" s="2" t="inlineStr">
+        <is>
+          <t>Recorded</t>
+        </is>
+      </c>
+      <c r="K4" s="4" t="inlineStr">
+        <is>
+          <t>Total Students</t>
+        </is>
+      </c>
+      <c r="L4" s="4" t="n">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>ANATOMY</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="E5" s="5" t="inlineStr">
+        <is>
+          <t>23/11/2025</t>
+        </is>
+      </c>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>12:00:00</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="inlineStr"/>
+      <c r="H5" s="5" t="inlineStr">
         <is>
           <t>0/251</t>
         </is>
       </c>
-      <c r="I4" s="4" t="inlineStr">
+      <c r="I5" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
       </c>
-      <c r="K4" s="5" t="inlineStr">
-        <is>
-          <t>Total Students</t>
-        </is>
-      </c>
-      <c r="L4" s="5" t="n">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B5" s="4" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C5" s="4" t="inlineStr">
+      <c r="K5" s="4" t="inlineStr">
+        <is>
+          <t>Total Sessions</t>
+        </is>
+      </c>
+      <c r="L5" s="4" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
         <is>
           <t>ANATOMY</t>
         </is>
       </c>
-      <c r="D5" s="4" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
-      </c>
-      <c r="E5" s="4" t="inlineStr">
-        <is>
-          <t>23/11/2025</t>
-        </is>
-      </c>
-      <c r="F5" s="4" t="inlineStr">
-        <is>
-          <t>12:00:00</t>
-        </is>
-      </c>
-      <c r="G5" s="4" t="inlineStr"/>
-      <c r="H5" s="4" t="inlineStr">
+      <c r="D6" s="5" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="E6" s="5" t="inlineStr">
+        <is>
+          <t>30/11/2025</t>
+        </is>
+      </c>
+      <c r="F6" s="5" t="inlineStr">
+        <is>
+          <t>14:00:00</t>
+        </is>
+      </c>
+      <c r="G6" s="5" t="inlineStr"/>
+      <c r="H6" s="5" t="inlineStr">
         <is>
           <t>0/251</t>
         </is>
       </c>
-      <c r="I5" s="4" t="inlineStr">
+      <c r="I6" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
       </c>
-      <c r="K5" s="5" t="inlineStr">
-        <is>
-          <t>Total Sessions</t>
-        </is>
-      </c>
-      <c r="L5" s="5" t="n">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B6" s="4" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C6" s="4" t="inlineStr">
-        <is>
-          <t>ANATOMY</t>
-        </is>
-      </c>
-      <c r="D6" s="4" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="E6" s="4" t="inlineStr">
-        <is>
-          <t>30/11/2025</t>
-        </is>
-      </c>
-      <c r="F6" s="4" t="inlineStr">
-        <is>
-          <t>14:00:00</t>
-        </is>
-      </c>
-      <c r="G6" s="4" t="inlineStr"/>
-      <c r="H6" s="4" t="inlineStr">
+      <c r="K6" s="4" t="inlineStr">
+        <is>
+          <t>Recorded Sessions</t>
+        </is>
+      </c>
+      <c r="L6" s="4" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="5" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C7" s="5" t="inlineStr">
+        <is>
+          <t>BIOCHEMISTRY LAB/CBL</t>
+        </is>
+      </c>
+      <c r="D7" s="5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="E7" s="5" t="inlineStr">
+        <is>
+          <t>19/11/2025</t>
+        </is>
+      </c>
+      <c r="F7" s="5" t="inlineStr">
+        <is>
+          <t>10:00:00</t>
+        </is>
+      </c>
+      <c r="G7" s="5" t="inlineStr"/>
+      <c r="H7" s="5" t="inlineStr">
         <is>
           <t>0/251</t>
         </is>
       </c>
-      <c r="I6" s="4" t="inlineStr">
+      <c r="I7" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
       </c>
-      <c r="K6" s="5" t="inlineStr">
-        <is>
-          <t>Recorded Sessions</t>
-        </is>
-      </c>
-      <c r="L6" s="5" t="n">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B7" s="4" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C7" s="4" t="inlineStr">
+      <c r="K7" s="4" t="inlineStr">
+        <is>
+          <t>Missing Sessions</t>
+        </is>
+      </c>
+      <c r="L7" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="5" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B8" s="5" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C8" s="5" t="inlineStr">
         <is>
           <t>BIOCHEMISTRY LAB/CBL</t>
         </is>
       </c>
-      <c r="D7" s="4" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="E7" s="4" t="inlineStr">
-        <is>
-          <t>19/11/2025</t>
-        </is>
-      </c>
-      <c r="F7" s="4" t="inlineStr">
-        <is>
-          <t>10:00:00</t>
-        </is>
-      </c>
-      <c r="G7" s="4" t="inlineStr"/>
-      <c r="H7" s="4" t="inlineStr">
+      <c r="D8" s="5" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E8" s="5" t="inlineStr">
+        <is>
+          <t>27/11/2025</t>
+        </is>
+      </c>
+      <c r="F8" s="5" t="inlineStr">
+        <is>
+          <t>08:00:00</t>
+        </is>
+      </c>
+      <c r="G8" s="5" t="inlineStr"/>
+      <c r="H8" s="5" t="inlineStr">
         <is>
           <t>0/251</t>
         </is>
       </c>
-      <c r="I7" s="4" t="inlineStr">
+      <c r="I8" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
       </c>
-      <c r="K7" s="5" t="inlineStr">
-        <is>
-          <t>Missing Sessions</t>
-        </is>
-      </c>
-      <c r="L7" s="5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B8" s="4" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C8" s="4" t="inlineStr">
-        <is>
-          <t>BIOCHEMISTRY LAB/CBL</t>
-        </is>
-      </c>
-      <c r="D8" s="4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E8" s="4" t="inlineStr">
-        <is>
-          <t>27/11/2025</t>
-        </is>
-      </c>
-      <c r="F8" s="4" t="inlineStr">
-        <is>
-          <t>08:00:00</t>
-        </is>
-      </c>
-      <c r="G8" s="4" t="inlineStr"/>
-      <c r="H8" s="4" t="inlineStr">
-        <is>
-          <t>0/251</t>
-        </is>
-      </c>
-      <c r="I8" s="4" t="inlineStr">
-        <is>
-          <t>Pending</t>
-        </is>
-      </c>
-      <c r="K8" s="5" t="inlineStr">
+      <c r="K8" s="4" t="inlineStr">
         <is>
           <t>Pending Sessions</t>
         </is>
       </c>
-      <c r="L8" s="5" t="n">
-        <v>20</v>
+      <c r="L8" s="4" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="9">
@@ -958,14 +962,14 @@
           <t>Recorded</t>
         </is>
       </c>
-      <c r="K9" s="5" t="inlineStr">
+      <c r="K9" s="4" t="inlineStr">
         <is>
           <t>Coverage %</t>
         </is>
       </c>
-      <c r="L9" s="5" t="inlineStr">
-        <is>
-          <t>27.6%</t>
+      <c r="L9" s="4" t="inlineStr">
+        <is>
+          <t>31.0%</t>
         </is>
       </c>
     </row>
@@ -1015,141 +1019,141 @@
           <t>Recorded</t>
         </is>
       </c>
-      <c r="K10" s="5" t="inlineStr">
+      <c r="K10" s="4" t="inlineStr">
         <is>
           <t>Average Attendance %</t>
         </is>
       </c>
-      <c r="L10" s="5" t="inlineStr">
-        <is>
-          <t>25.0%</t>
+      <c r="L10" s="4" t="inlineStr">
+        <is>
+          <t>22.9%</t>
         </is>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B11" s="4" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C11" s="4" t="inlineStr">
+      <c r="A11" s="5" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B11" s="5" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C11" s="5" t="inlineStr">
         <is>
           <t>HISTOLOGY</t>
         </is>
       </c>
-      <c r="D11" s="4" t="inlineStr">
+      <c r="D11" s="5" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="E11" s="4" t="inlineStr">
+      <c r="E11" s="5" t="inlineStr">
         <is>
           <t>01/12/2025</t>
         </is>
       </c>
-      <c r="F11" s="4" t="inlineStr">
+      <c r="F11" s="5" t="inlineStr">
         <is>
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G11" s="4" t="inlineStr"/>
-      <c r="H11" s="4" t="inlineStr">
+      <c r="G11" s="5" t="inlineStr"/>
+      <c r="H11" s="5" t="inlineStr">
         <is>
           <t>0/251</t>
         </is>
       </c>
-      <c r="I11" s="4" t="inlineStr">
+      <c r="I11" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B12" s="4" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C12" s="4" t="inlineStr">
+      <c r="A12" s="5" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B12" s="5" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C12" s="5" t="inlineStr">
         <is>
           <t>MICROBIOLOGY</t>
         </is>
       </c>
-      <c r="D12" s="4" t="inlineStr">
+      <c r="D12" s="5" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E12" s="4" t="inlineStr">
+      <c r="E12" s="5" t="inlineStr">
         <is>
           <t>24/11/2025</t>
         </is>
       </c>
-      <c r="F12" s="4" t="inlineStr">
+      <c r="F12" s="5" t="inlineStr">
         <is>
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G12" s="4" t="inlineStr"/>
-      <c r="H12" s="4" t="inlineStr">
+      <c r="G12" s="5" t="inlineStr"/>
+      <c r="H12" s="5" t="inlineStr">
         <is>
           <t>0/251</t>
         </is>
       </c>
-      <c r="I12" s="4" t="inlineStr">
+      <c r="I12" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B13" s="4" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C13" s="4" t="inlineStr">
+      <c r="A13" s="5" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
         <is>
           <t>MICROBIOLOGY</t>
         </is>
       </c>
-      <c r="D13" s="4" t="inlineStr">
+      <c r="D13" s="5" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E13" s="4" t="inlineStr">
+      <c r="E13" s="5" t="inlineStr">
         <is>
           <t>10/12/2025</t>
         </is>
       </c>
-      <c r="F13" s="4" t="inlineStr">
+      <c r="F13" s="5" t="inlineStr">
         <is>
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G13" s="4" t="inlineStr"/>
-      <c r="H13" s="4" t="inlineStr">
+      <c r="G13" s="5" t="inlineStr"/>
+      <c r="H13" s="5" t="inlineStr">
         <is>
           <t>0/251</t>
         </is>
       </c>
-      <c r="I13" s="4" t="inlineStr">
+      <c r="I13" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
@@ -1298,166 +1302,166 @@
           <t>Recorded</t>
         </is>
       </c>
-      <c r="K15" s="5" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="L15" s="5" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="M15" s="5" t="n">
+      <c r="K15" s="4" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="L15" s="4" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="M15" s="4" t="n">
         <v>251</v>
       </c>
-      <c r="N15" s="5" t="n">
+      <c r="N15" s="4" t="n">
         <v>29</v>
       </c>
-      <c r="O15" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="P15" s="5" t="n">
+      <c r="O15" s="4" t="n">
+        <v>9</v>
+      </c>
+      <c r="P15" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="Q15" s="5" t="n">
-        <v>20</v>
-      </c>
-      <c r="R15" s="5" t="inlineStr">
-        <is>
-          <t>27.6%</t>
-        </is>
-      </c>
-      <c r="S15" s="5" t="inlineStr">
-        <is>
-          <t>25.0%</t>
+      <c r="Q15" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="R15" s="4" t="inlineStr">
+        <is>
+          <t>31.0%</t>
+        </is>
+      </c>
+      <c r="S15" s="4" t="inlineStr">
+        <is>
+          <t>22.9%</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B16" s="4" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C16" s="4" t="inlineStr">
+      <c r="A16" s="5" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B16" s="5" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C16" s="5" t="inlineStr">
         <is>
           <t>PARASITOLOGY</t>
         </is>
       </c>
-      <c r="D16" s="4" t="inlineStr">
+      <c r="D16" s="5" t="inlineStr">
         <is>
           <t>4</t>
         </is>
       </c>
-      <c r="E16" s="4" t="inlineStr">
+      <c r="E16" s="5" t="inlineStr">
         <is>
           <t>30/11/2025</t>
         </is>
       </c>
-      <c r="F16" s="4" t="inlineStr">
+      <c r="F16" s="5" t="inlineStr">
         <is>
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G16" s="4" t="inlineStr"/>
-      <c r="H16" s="4" t="inlineStr">
+      <c r="G16" s="5" t="inlineStr"/>
+      <c r="H16" s="5" t="inlineStr">
         <is>
           <t>0/251</t>
         </is>
       </c>
-      <c r="I16" s="4" t="inlineStr">
+      <c r="I16" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B17" s="4" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C17" s="4" t="inlineStr">
+      <c r="A17" s="5" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C17" s="5" t="inlineStr">
         <is>
           <t>PARASITOLOGY</t>
         </is>
       </c>
-      <c r="D17" s="4" t="inlineStr">
+      <c r="D17" s="5" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="E17" s="4" t="inlineStr">
+      <c r="E17" s="5" t="inlineStr">
         <is>
           <t>03/12/2025</t>
         </is>
       </c>
-      <c r="F17" s="4" t="inlineStr">
+      <c r="F17" s="5" t="inlineStr">
         <is>
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G17" s="4" t="inlineStr"/>
-      <c r="H17" s="4" t="inlineStr">
+      <c r="G17" s="5" t="inlineStr"/>
+      <c r="H17" s="5" t="inlineStr">
         <is>
           <t>0/251</t>
         </is>
       </c>
-      <c r="I17" s="4" t="inlineStr">
+      <c r="I17" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B18" s="4" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C18" s="4" t="inlineStr">
+      <c r="A18" s="5" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B18" s="5" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
         <is>
           <t>PARASITOLOGY</t>
         </is>
       </c>
-      <c r="D18" s="4" t="inlineStr">
+      <c r="D18" s="5" t="inlineStr">
         <is>
           <t>6</t>
         </is>
       </c>
-      <c r="E18" s="4" t="inlineStr">
+      <c r="E18" s="5" t="inlineStr">
         <is>
           <t>08/12/2025</t>
         </is>
       </c>
-      <c r="F18" s="4" t="inlineStr">
+      <c r="F18" s="5" t="inlineStr">
         <is>
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G18" s="4" t="inlineStr"/>
-      <c r="H18" s="4" t="inlineStr">
+      <c r="G18" s="5" t="inlineStr"/>
+      <c r="H18" s="5" t="inlineStr">
         <is>
           <t>0/251</t>
         </is>
       </c>
-      <c r="I18" s="4" t="inlineStr">
+      <c r="I18" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
@@ -1469,43 +1473,43 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B19" s="4" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C19" s="4" t="inlineStr">
+      <c r="A19" s="5" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B19" s="5" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C19" s="5" t="inlineStr">
         <is>
           <t>PARASITOLOGY</t>
         </is>
       </c>
-      <c r="D19" s="4" t="inlineStr">
+      <c r="D19" s="5" t="inlineStr">
         <is>
           <t>7</t>
         </is>
       </c>
-      <c r="E19" s="4" t="inlineStr">
+      <c r="E19" s="5" t="inlineStr">
         <is>
           <t>10/12/2025</t>
         </is>
       </c>
-      <c r="F19" s="4" t="inlineStr">
+      <c r="F19" s="5" t="inlineStr">
         <is>
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G19" s="4" t="inlineStr"/>
-      <c r="H19" s="4" t="inlineStr">
+      <c r="G19" s="5" t="inlineStr"/>
+      <c r="H19" s="5" t="inlineStr">
         <is>
           <t>0/251</t>
         </is>
       </c>
-      <c r="I19" s="4" t="inlineStr">
+      <c r="I19" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
@@ -1527,48 +1531,48 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B20" s="4" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C20" s="4" t="inlineStr">
+      <c r="A20" s="5" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B20" s="5" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C20" s="5" t="inlineStr">
         <is>
           <t>PARASITOLOGY SGD/POS</t>
         </is>
       </c>
-      <c r="D20" s="4" t="inlineStr">
+      <c r="D20" s="5" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E20" s="4" t="inlineStr">
+      <c r="E20" s="5" t="inlineStr">
         <is>
           <t>09/12/2025</t>
         </is>
       </c>
-      <c r="F20" s="4" t="inlineStr">
+      <c r="F20" s="5" t="inlineStr">
         <is>
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G20" s="4" t="inlineStr"/>
-      <c r="H20" s="4" t="inlineStr">
+      <c r="G20" s="5" t="inlineStr"/>
+      <c r="H20" s="5" t="inlineStr">
         <is>
           <t>0/251</t>
         </is>
       </c>
-      <c r="I20" s="4" t="inlineStr">
+      <c r="I20" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
       </c>
-      <c r="K20" s="5" t="inlineStr">
+      <c r="K20" s="4" t="inlineStr">
         <is>
           <t>Recorded</t>
         </is>
@@ -1578,55 +1582,55 @@
           <t>Green</t>
         </is>
       </c>
-      <c r="M20" s="5" t="inlineStr">
+      <c r="M20" s="4" t="inlineStr">
         <is>
           <t>Session recorded</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B21" s="4" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C21" s="4" t="inlineStr">
+      <c r="A21" s="5" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B21" s="5" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C21" s="5" t="inlineStr">
         <is>
           <t>PARASITOLOGY SGD/POS</t>
         </is>
       </c>
-      <c r="D21" s="4" t="inlineStr">
+      <c r="D21" s="5" t="inlineStr">
         <is>
           <t>5</t>
         </is>
       </c>
-      <c r="E21" s="4" t="inlineStr">
+      <c r="E21" s="5" t="inlineStr">
         <is>
           <t>03/12/2025</t>
         </is>
       </c>
-      <c r="F21" s="4" t="inlineStr">
+      <c r="F21" s="5" t="inlineStr">
         <is>
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G21" s="4" t="inlineStr"/>
-      <c r="H21" s="4" t="inlineStr">
+      <c r="G21" s="5" t="inlineStr"/>
+      <c r="H21" s="5" t="inlineStr">
         <is>
           <t>0/251</t>
         </is>
       </c>
-      <c r="I21" s="4" t="inlineStr">
+      <c r="I21" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
       </c>
-      <c r="K21" s="5" t="inlineStr">
+      <c r="K21" s="4" t="inlineStr">
         <is>
           <t>Not Recorded</t>
         </is>
@@ -1636,55 +1640,55 @@
           <t>Red</t>
         </is>
       </c>
-      <c r="M21" s="5" t="inlineStr">
+      <c r="M21" s="4" t="inlineStr">
         <is>
           <t>Session missed</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B22" s="4" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C22" s="4" t="inlineStr">
+      <c r="A22" s="5" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B22" s="5" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
         <is>
           <t>PATHOLOGY LAB/MUSEUM</t>
         </is>
       </c>
-      <c r="D22" s="4" t="inlineStr">
+      <c r="D22" s="5" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E22" s="4" t="inlineStr">
+      <c r="E22" s="5" t="inlineStr">
         <is>
           <t>26/11/2025</t>
         </is>
       </c>
-      <c r="F22" s="4" t="inlineStr">
+      <c r="F22" s="5" t="inlineStr">
         <is>
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G22" s="4" t="inlineStr"/>
-      <c r="H22" s="4" t="inlineStr">
+      <c r="G22" s="5" t="inlineStr"/>
+      <c r="H22" s="5" t="inlineStr">
         <is>
           <t>0/251</t>
         </is>
       </c>
-      <c r="I22" s="4" t="inlineStr">
+      <c r="I22" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
       </c>
-      <c r="K22" s="5" t="inlineStr">
+      <c r="K22" s="4" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
@@ -1694,136 +1698,136 @@
           <t>Yellow</t>
         </is>
       </c>
-      <c r="M22" s="5" t="inlineStr">
+      <c r="M22" s="4" t="inlineStr">
         <is>
           <t>Future session</t>
         </is>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B23" s="4" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C23" s="4" t="inlineStr">
+      <c r="A23" s="5" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B23" s="5" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C23" s="5" t="inlineStr">
         <is>
           <t>PATHOLOGY LAB/MUSEUM</t>
         </is>
       </c>
-      <c r="D23" s="4" t="inlineStr">
+      <c r="D23" s="5" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E23" s="4" t="inlineStr">
+      <c r="E23" s="5" t="inlineStr">
         <is>
           <t>27/11/2025</t>
         </is>
       </c>
-      <c r="F23" s="4" t="inlineStr">
+      <c r="F23" s="5" t="inlineStr">
         <is>
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G23" s="4" t="inlineStr"/>
-      <c r="H23" s="4" t="inlineStr">
+      <c r="G23" s="5" t="inlineStr"/>
+      <c r="H23" s="5" t="inlineStr">
         <is>
           <t>0/251</t>
         </is>
       </c>
-      <c r="I23" s="4" t="inlineStr">
+      <c r="I23" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B24" s="4" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C24" s="4" t="inlineStr">
+      <c r="A24" s="5" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C24" s="5" t="inlineStr">
         <is>
           <t>PATHOLOGY LAB/MUSEUM</t>
         </is>
       </c>
-      <c r="D24" s="4" t="inlineStr">
+      <c r="D24" s="5" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E24" s="4" t="inlineStr">
+      <c r="E24" s="5" t="inlineStr">
         <is>
           <t>07/12/2025</t>
         </is>
       </c>
-      <c r="F24" s="4" t="inlineStr">
+      <c r="F24" s="5" t="inlineStr">
         <is>
           <t>12:00:00</t>
         </is>
       </c>
-      <c r="G24" s="4" t="inlineStr"/>
-      <c r="H24" s="4" t="inlineStr">
+      <c r="G24" s="5" t="inlineStr"/>
+      <c r="H24" s="5" t="inlineStr">
         <is>
           <t>0/251</t>
         </is>
       </c>
-      <c r="I24" s="4" t="inlineStr">
+      <c r="I24" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B25" s="4" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C25" s="4" t="inlineStr">
+      <c r="A25" s="5" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B25" s="5" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C25" s="5" t="inlineStr">
         <is>
           <t>PATHOLOGY LAB/MUSEUM</t>
         </is>
       </c>
-      <c r="D25" s="4" t="inlineStr">
+      <c r="D25" s="5" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E25" s="4" t="inlineStr">
+      <c r="E25" s="5" t="inlineStr">
         <is>
           <t>08/12/2025</t>
         </is>
       </c>
-      <c r="F25" s="4" t="inlineStr">
+      <c r="F25" s="5" t="inlineStr">
         <is>
           <t>08:00:00</t>
         </is>
       </c>
-      <c r="G25" s="4" t="inlineStr"/>
-      <c r="H25" s="4" t="inlineStr">
+      <c r="G25" s="5" t="inlineStr"/>
+      <c r="H25" s="5" t="inlineStr">
         <is>
           <t>0/251</t>
         </is>
       </c>
-      <c r="I25" s="4" t="inlineStr">
+      <c r="I25" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
@@ -1877,43 +1881,43 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B27" s="4" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C27" s="4" t="inlineStr">
+      <c r="A27" s="5" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B27" s="5" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C27" s="5" t="inlineStr">
         <is>
           <t>PHARMACOLOGY</t>
         </is>
       </c>
-      <c r="D27" s="4" t="inlineStr">
+      <c r="D27" s="5" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E27" s="4" t="inlineStr">
+      <c r="E27" s="5" t="inlineStr">
         <is>
           <t>24/11/2025</t>
         </is>
       </c>
-      <c r="F27" s="4" t="inlineStr">
+      <c r="F27" s="5" t="inlineStr">
         <is>
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G27" s="4" t="inlineStr"/>
-      <c r="H27" s="4" t="inlineStr">
+      <c r="G27" s="5" t="inlineStr"/>
+      <c r="H27" s="5" t="inlineStr">
         <is>
           <t>0/251</t>
         </is>
       </c>
-      <c r="I27" s="4" t="inlineStr">
+      <c r="I27" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>
@@ -1952,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">
@@ -2010,43 +2014,43 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B30" s="4" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C30" s="4" t="inlineStr">
+      <c r="A30" s="5" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B30" s="5" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C30" s="5" t="inlineStr">
         <is>
           <t>PHYSIOLOGY</t>
         </is>
       </c>
-      <c r="D30" s="4" t="inlineStr">
+      <c r="D30" s="5" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="E30" s="4" t="inlineStr">
+      <c r="E30" s="5" t="inlineStr">
         <is>
           <t>02/12/2025</t>
         </is>
       </c>
-      <c r="F30" s="4" t="inlineStr">
+      <c r="F30" s="5" t="inlineStr">
         <is>
           <t>11:00:00</t>
         </is>
       </c>
-      <c r="G30" s="4" t="inlineStr"/>
-      <c r="H30" s="4" t="inlineStr">
+      <c r="G30" s="5" t="inlineStr"/>
+      <c r="H30" s="5" t="inlineStr">
         <is>
           <t>0/251</t>
         </is>
       </c>
-      <c r="I30" s="4" t="inlineStr">
+      <c r="I30" s="5" t="inlineStr">
         <is>
           <t>Pending</t>
         </is>

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-17 10:17:44
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>System, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>eman.tantawi@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>System, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-17 11:13:17
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>System, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
+          <t>System, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-17 12:31:01
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>System, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>System, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-17 13:28:18
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-17 14:15:07
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-17 15:17:04
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System</t>
+          <t>asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-17 17:15:03
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>System, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>System, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-17 20:17:00
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-17 21:13:26
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, System</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System</t>
+          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-17 22:14:10
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, servinaz@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-17 23:13:54
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-18 01:09:56
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System</t>
+          <t>Veronia.rafat@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-18 03:08:23
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-18 04:18:40
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System</t>
+          <t>Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-18 05:15:00
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System</t>
+          <t>System, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg</t>
+          <t>eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-18 06:22:21
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-18 07:14:45
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-18 08:20:38
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>System, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>System, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-18 09:17:07
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-18 10:18:11
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System</t>
+          <t>asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-18 11:13:43
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, servinaz@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-18 12:31:36
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, System</t>
+          <t>Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
+          <t>Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-18 13:28:33
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg</t>
+          <t>System, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-18 14:15:03
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-18 15:16:56
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-18 16:20:24
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg</t>
+          <t>System, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
+          <t>System, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-18 17:14:48
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-18 18:22:15
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-18 19:12:48
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>System, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-18 20:18:14
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>System, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>System, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-18 22:14:30
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-18 23:13:55
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-19 01:09:34
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System</t>
+          <t>hend_mahmoud@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-19 03:07:36
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-19 04:18:35
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-19 05:15:34
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-19 06:21:59
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-19 07:15:11
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>System, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System</t>
+          <t>eman.tantawi@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-19 08:20:10
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>System, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>eman.tantawi@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-19 09:17:29
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -96,6 +96,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -103,9 +106,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -815,45 +815,45 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="5" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B7" s="5" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C7" s="5" t="inlineStr">
+      <c r="A7" s="6" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C7" s="6" t="inlineStr">
         <is>
           <t>BIOCHEMISTRY LAB/CBL</t>
         </is>
       </c>
-      <c r="D7" s="5" t="inlineStr">
+      <c r="D7" s="6" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E7" s="5" t="inlineStr">
+      <c r="E7" s="6" t="inlineStr">
         <is>
           <t>19/11/2025</t>
         </is>
       </c>
-      <c r="F7" s="5" t="inlineStr">
+      <c r="F7" s="6" t="inlineStr">
         <is>
           <t>10:00:00</t>
         </is>
       </c>
-      <c r="G7" s="5" t="inlineStr"/>
-      <c r="H7" s="5" t="inlineStr">
+      <c r="G7" s="6" t="inlineStr"/>
+      <c r="H7" s="6" t="inlineStr">
         <is>
           <t>0/251</t>
         </is>
       </c>
-      <c r="I7" s="5" t="inlineStr">
-        <is>
-          <t>Pending</t>
+      <c r="I7" s="6" t="inlineStr">
+        <is>
+          <t>Not Recorded</t>
         </is>
       </c>
       <c r="K7" s="4" t="inlineStr">
@@ -862,7 +862,7 @@
         </is>
       </c>
       <c r="L7" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8">
@@ -913,7 +913,7 @@
         </is>
       </c>
       <c r="L8" s="4" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1322,10 +1322,10 @@
         <v>9</v>
       </c>
       <c r="P15" s="4" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q15" s="4" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="R15" s="4" t="inlineStr">
         <is>
@@ -1577,7 +1577,7 @@
           <t>Recorded</t>
         </is>
       </c>
-      <c r="L20" s="6" t="inlineStr">
+      <c r="L20" s="7" t="inlineStr">
         <is>
           <t>Green</t>
         </is>
@@ -1635,7 +1635,7 @@
           <t>Not Recorded</t>
         </is>
       </c>
-      <c r="L21" s="7" t="inlineStr">
+      <c r="L21" s="8" t="inlineStr">
         <is>
           <t>Red</t>
         </is>
@@ -1693,7 +1693,7 @@
           <t>Pending</t>
         </is>
       </c>
-      <c r="L22" s="8" t="inlineStr">
+      <c r="L22" s="9" t="inlineStr">
         <is>
           <t>Yellow</t>
         </is>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">
@@ -1971,43 +1971,43 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="9" t="inlineStr">
-        <is>
-          <t>Year 2</t>
-        </is>
-      </c>
-      <c r="B29" s="9" t="inlineStr">
-        <is>
-          <t>C1</t>
-        </is>
-      </c>
-      <c r="C29" s="9" t="inlineStr">
+      <c r="A29" s="6" t="inlineStr">
+        <is>
+          <t>Year 2</t>
+        </is>
+      </c>
+      <c r="B29" s="6" t="inlineStr">
+        <is>
+          <t>C1</t>
+        </is>
+      </c>
+      <c r="C29" s="6" t="inlineStr">
         <is>
           <t>PHYSIOLOGY</t>
         </is>
       </c>
-      <c r="D29" s="9" t="inlineStr">
+      <c r="D29" s="6" t="inlineStr">
         <is>
           <t>2</t>
         </is>
       </c>
-      <c r="E29" s="9" t="inlineStr">
+      <c r="E29" s="6" t="inlineStr">
         <is>
           <t>16/11/2025</t>
         </is>
       </c>
-      <c r="F29" s="9" t="inlineStr">
+      <c r="F29" s="6" t="inlineStr">
         <is>
           <t>14:00:00</t>
         </is>
       </c>
-      <c r="G29" s="9" t="inlineStr"/>
-      <c r="H29" s="9" t="inlineStr">
+      <c r="G29" s="6" t="inlineStr"/>
+      <c r="H29" s="6" t="inlineStr">
         <is>
           <t>0/251</t>
         </is>
       </c>
-      <c r="I29" s="9" t="inlineStr">
+      <c r="I29" s="6" t="inlineStr">
         <is>
           <t>Not Recorded</t>
         </is>

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-19 10:16:46
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-19 11:13:14
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-19 12:30:52
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System</t>
+          <t>Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System</t>
+          <t>Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-19 13:28:24
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -949,7 +949,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1289,7 +1289,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-19 15:16:32
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
+          <t>AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-19 16:20:14
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System</t>
+          <t>System, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
+          <t>System, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
+          <t>menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-19 17:14:41
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>System, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
+          <t>Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-19 18:21:47
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
+          <t>AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-19 19:12:23
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-19 20:15:00
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System</t>
+          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
+          <t>lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-19 21:11:41
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg</t>
+          <t>System, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System</t>
+          <t>System, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
+          <t>Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-19 22:14:22
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
+          <t>Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-19 23:14:21
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
+          <t>servinaz@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System</t>
+          <t>System, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
+          <t>lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-20 01:08:08
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
+          <t>Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-20 03:05:55
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
+          <t>Veronia.rafat@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
+          <t>Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-20 04:17:10
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
+          <t>menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-20 05:15:15
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
+          <t>AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-20 06:22:04
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
+          <t>eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
+          <t>Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-20 07:14:53
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
+          <t>Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-20 08:21:01
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
+          <t>AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-20 09:16:10
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
+          <t>eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
+          <t>Fatmaelhady@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-20 10:16:31
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Fatmaelhady@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
+          <t>AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-20 11:13:33
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
+          <t>AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-20 12:30:10
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
+          <t>lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-20 13:26:37
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg</t>
+          <t>System, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
+          <t>AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-20 14:14:50
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
+          <t>AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-20 15:15:56
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
+          <t>Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-20 16:19:24
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, servinaz@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
+          <t>menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-20 17:12:10
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>System, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
+          <t>lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-20 18:21:53
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
+          <t>Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-20 19:11:58
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System</t>
+          <t>servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System</t>
+          <t>asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
+          <t>lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-20 20:17:32
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
+          <t>lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-20 21:14:02
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, servinaz@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
+          <t>lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-20 22:14:13
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
+          <t>Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-20 23:13:50
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
+          <t>menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-21 01:09:05
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
+          <t>Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-21 03:06:50
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
+          <t>AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-21 04:18:23
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
+          <t>AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-21 05:15:40
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, System</t>
+          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System</t>
+          <t>eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
+          <t>Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-21 06:23:37
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
+          <t>servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System</t>
+          <t>asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
+          <t>Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-21 07:15:16
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
+          <t>System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
+          <t>eman.tantawi@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
+          <t>lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-21 08:21:21
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>eman.tantawi@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
+          <t>Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-21 09:16:25
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, System</t>
+          <t>Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System</t>
+          <t>hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
+          <t>lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-21 10:15:53
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System</t>
+          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
+          <t>menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-21 11:12:40
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System</t>
+          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
+          <t>lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-21 12:29:04
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
+          <t>Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-21 13:24:49
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, System</t>
+          <t>System, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System</t>
+          <t>eman.tantawi@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
+          <t>AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-21 14:14:52
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>eman.tantawi@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
+          <t>Fatmaelhady@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-21 15:14:10
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>System, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Fatmaelhady@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
+          <t>Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-21 16:19:01
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
+          <t>lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-21 17:13:19
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
+          <t>AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-21 18:20:29
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System</t>
+          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
+          <t>lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-21 19:12:44
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
+          <t>Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-21 20:17:06
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg</t>
+          <t>System, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
+          <t>AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-21 21:13:25
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
+          <t>AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-21 22:14:26
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
+          <t>menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-21 23:13:21
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>System, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
+          <t>Fatmaelhady@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-22 01:06:24
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Fatmaelhady@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
+          <t>Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-22 03:00:07
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
+          <t>gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System</t>
+          <t>Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
+          <t>Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-22 04:17:07
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>System, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
+          <t>Kerelos.zareef@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-22 05:14:05
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>System, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
+          <t>System, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Kerelos.zareef@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
+          <t>lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-22 06:20:00
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
+          <t>Kerelos.zareef@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-22 07:13:14
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, servinaz@med.asu.edu.eg</t>
+          <t>System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>System, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Kerelos.zareef@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
+          <t>lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-22 08:18:25
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
+          <t>Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-22 09:13:58
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
+          <t>Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-22 10:14:20
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
+          <t>System, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
+          <t>lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-22 11:11:04
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>eman.tantawi@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
+          <t>Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-22 12:25:49
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>eman.tantawi@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
+          <t>menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-22 13:20:05
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
+          <t>AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-22 14:12:13
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
+          <t>menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-22 15:13:04
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, servinaz@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
+          <t>Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-22 16:16:21
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
+          <t>lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-22 17:11:57
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
+          <t>Kerelos.zareef@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-22 18:19:29
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, System, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Kerelos.zareef@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
+          <t>Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-22 19:10:52
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
+          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
+          <t>Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
+          <t>menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-22 20:15:26
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, System</t>
+          <t>System, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg</t>
+          <t>System, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
+          <t>menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-22 21:12:20
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
+          <t>menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-22 22:13:28
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System</t>
+          <t>System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg</t>
+          <t>eman.tantawi@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
+          <t>AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-22 23:13:50
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>eman.tantawi@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg</t>
+          <t>lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-23 01:18:42
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>System, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
+          <t>lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-23 03:23:09
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
+          <t>Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-23 04:28:56
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>System, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg</t>
+          <t>System, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg</t>
+          <t>lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-23 05:13:59
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>System, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
+          <t>Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-23 06:21:14
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System, majorelle.magdy@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Fatmaelhady@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
+          <t>menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-23 07:13:33
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, System, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg</t>
+          <t>Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System, asmaa.reda@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, servinaz@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg</t>
+          <t>menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
+          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
+          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-23 08:18:43
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, System, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, System</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>menna-alah.mohamed@asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
+          <t>AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
+          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="G15" s="2" t="inlineStr">
         <is>
-          <t>Rania.a.youssef@med.asu.edu.eg, mohamed.saleem@med.asu.edu.eg</t>
+          <t>mohamed.saleem@med.asu.edu.eg, Rania.a.youssef@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H15" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-23 09:14:15
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>Veronia.rafat@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, servinaz@med.asu.edu.eg, System</t>
+          <t>System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, System, hend_mahmoud@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, servinaz@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg</t>
+          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>AbeerRagheb@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg</t>
+          <t>Fatmaelhady@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -953,7 +953,7 @@
       </c>
       <c r="G9" s="2" t="inlineStr">
         <is>
-          <t>Shimaa.ashraf@med.asu.edu.eg, Safa.hany@med.asu.edu.eg</t>
+          <t>Safa.hany@med.asu.edu.eg, Shimaa.ashraf@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H9" s="2" t="inlineStr">

</xml_diff>

<commit_message>
Sync attendance_reports, modules_schedules, and assets from main repo - 2025-11-23 10:14:13
</commit_message>
<xml_diff>
--- a/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
+++ b/attendance_reports/Y2_B2526_GIT_&_Liver_session_analysis.xlsx
@@ -581,7 +581,7 @@
       </c>
       <c r="G2" s="2" t="inlineStr">
         <is>
-          <t>System, Amira.Sobhy@med.asu.edu.eg, gehanadel@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg, servinaz@med.asu.edu.eg</t>
+          <t>System, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, Amira.Sobhy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H2" s="2" t="inlineStr">
@@ -633,7 +633,7 @@
       </c>
       <c r="G3" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, System, Veronia.rafat@med.asu.edu.eg, eman.tantawi@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>System, eman.tantawi@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg, Veronia.rafat@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H3" s="2" t="inlineStr">
@@ -690,7 +690,7 @@
       </c>
       <c r="G4" s="2" t="inlineStr">
         <is>
-          <t>majorelle.magdy@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, gehanadel@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg</t>
+          <t>gehanadel@med.asu.edu.eg, hend_mahmoud@med.asu.edu.eg, servinaz@med.asu.edu.eg, asmaa.reda@med.asu.edu.eg, majorelle.magdy@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H4" s="2" t="inlineStr">
@@ -847,7 +847,7 @@
       </c>
       <c r="G7" s="2" t="inlineStr">
         <is>
-          <t>Fatmaelhady@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Kerelos.zareef@med.asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
+          <t>Kerelos.zareef@med.asu.edu.eg, lamiaa.ossama@med.asu.edu.eg, Fatmaelhady@med.asu.edu.eg, menna-alah.mohamed@asu.edu.eg, AbeerRagheb@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H7" s="2" t="inlineStr">
@@ -1960,7 +1960,7 @@
       </c>
       <c r="G28" s="2" t="inlineStr">
         <is>
-          <t>Aya_hamed@med.asu.edu.eg, maryam.ashraf@med.asu.edu.eg</t>
+          <t>maryam.ashraf@med.asu.edu.eg, Aya_hamed@med.asu.edu.eg</t>
         </is>
       </c>
       <c r="H28" s="2" t="inlineStr">

</xml_diff>